<commit_message>
ValenceMax.py created and smact_data.py updated
ValenceMin.py calculates valence band maximum for a given anion/cation
pair and smact_data.py updated to get covalent radii from chemlab.
smact_data.py should be updated to retrieve eigenvalues in
solid_properties.txt.
</commit_message>
<xml_diff>
--- a/solid_properties.xlsx
+++ b/solid_properties.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="1620" windowWidth="25600" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="25600" windowHeight="17780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Elements" localSheetId="0">Sheet1!$A$3:$C$241</definedName>
-    <definedName name="Elements_Radii" localSheetId="0">Sheet1!$D$2:$F$88</definedName>
+    <definedName name="Elements_Radii" localSheetId="0">Sheet1!$D$2:$F$91</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -47,10 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
-  <si>
-    <t>Ag</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="182">
   <si>
     <t>Silver</t>
   </si>
@@ -79,9 +76,6 @@
     <t>Astatine</t>
   </si>
   <si>
-    <t>Au</t>
-  </si>
-  <si>
     <t>Gold</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>Cesium</t>
   </si>
   <si>
-    <t>Cu</t>
-  </si>
-  <si>
     <t>Copper</t>
   </si>
   <si>
@@ -583,10 +574,25 @@
     <t>Covalent Radius (pm)</t>
   </si>
   <si>
-    <t>Ep</t>
-  </si>
-  <si>
-    <t>Ed</t>
+    <t>Cu(d)</t>
+  </si>
+  <si>
+    <t>Cu(p)</t>
+  </si>
+  <si>
+    <t>Ag(d)</t>
+  </si>
+  <si>
+    <t>Ag(p)</t>
+  </si>
+  <si>
+    <t>Au(d)</t>
+  </si>
+  <si>
+    <t>Au(p)</t>
+  </si>
+  <si>
+    <t>Eigenval</t>
   </si>
 </sst>
 </file>
@@ -643,8 +649,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,7 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -675,6 +707,19 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +728,19 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:F88"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1036,77 +1094,74 @@
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D4">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>90</v>
@@ -1115,15 +1170,15 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>82</v>
@@ -1132,15 +1187,15 @@
         <v>6.64</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>77</v>
@@ -1149,15 +1204,15 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8">
         <v>75</v>
@@ -1166,15 +1221,15 @@
         <v>11.47</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9">
         <v>73</v>
@@ -1183,15 +1238,15 @@
         <v>14.13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>72</v>
@@ -1200,15 +1255,15 @@
         <v>16.989999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D11">
         <v>71</v>
@@ -1217,29 +1272,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D12">
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D13">
         <v>136</v>
@@ -1248,15 +1303,15 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>118</v>
@@ -1265,15 +1320,15 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D15">
         <v>111.00000000000001</v>
@@ -1282,15 +1337,15 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D16">
         <v>106</v>
@@ -1299,15 +1354,15 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D17">
         <v>102</v>
@@ -1316,15 +1371,15 @@
         <v>10.27</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>99</v>
@@ -1333,15 +1388,15 @@
         <v>12.31</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>98</v>
@@ -1350,1119 +1405,1161 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>202.99999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21">
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D22">
         <v>144</v>
       </c>
-      <c r="F22">
+      <c r="E22">
         <v>9.35</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D23">
         <v>132</v>
       </c>
-      <c r="F23">
+      <c r="E23">
         <v>11.04</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D24">
         <v>122</v>
       </c>
-      <c r="F24">
+      <c r="E24">
         <v>12.55</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25">
         <v>118</v>
       </c>
-      <c r="F25">
+      <c r="E25">
         <v>13.94</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26">
         <v>117</v>
       </c>
-      <c r="F26">
+      <c r="E26">
         <v>15.27</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <v>117</v>
       </c>
-      <c r="F27">
+      <c r="E27">
         <v>16.54</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D28">
         <v>115.99999999999999</v>
       </c>
-      <c r="F28">
+      <c r="E28">
         <v>17.77</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D29">
         <v>114.99999999999999</v>
       </c>
-      <c r="F29">
+      <c r="E29">
         <v>18.96</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>175</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>117</v>
       </c>
       <c r="E30">
-        <v>1.83</v>
-      </c>
-      <c r="F30">
         <v>6.92</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>117</v>
+      </c>
+      <c r="E31">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32">
+        <v>125</v>
+      </c>
+      <c r="E32">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33">
+        <v>126</v>
+      </c>
+      <c r="E33">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>122</v>
+      </c>
+      <c r="E34">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>120</v>
+      </c>
+      <c r="E35">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36">
+        <v>115.99999999999999</v>
+      </c>
+      <c r="E36">
+        <v>9.5299999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37">
+        <v>113.99999999999999</v>
+      </c>
+      <c r="E37">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38">
+        <v>112.00000000000001</v>
+      </c>
+      <c r="E38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>138</v>
+      </c>
+      <c r="D40">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41">
+        <v>162</v>
+      </c>
+      <c r="E41">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>169</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
         <v>170</v>
       </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>171</v>
-      </c>
-      <c r="D31">
-        <v>125</v>
-      </c>
-      <c r="E31">
-        <v>3.38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32">
-        <v>126</v>
-      </c>
-      <c r="E32">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33">
+      <c r="D42">
+        <v>145</v>
+      </c>
+      <c r="E42">
+        <v>8.4600000000000009</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43">
+        <v>134</v>
+      </c>
+      <c r="E43">
+        <v>10.029999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44">
+        <v>130</v>
+      </c>
+      <c r="E44">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45">
+        <v>127</v>
+      </c>
+      <c r="E45">
+        <v>13.08</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
         <v>122</v>
-      </c>
-      <c r="E33">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34">
-        <v>120</v>
-      </c>
-      <c r="E34">
-        <v>7.91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35">
-        <v>115.99999999999999</v>
-      </c>
-      <c r="E35">
-        <v>9.5299999999999994</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36">
-        <v>113.99999999999999</v>
-      </c>
-      <c r="E36">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37">
-        <v>112.00000000000001</v>
-      </c>
-      <c r="E37">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40">
-        <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>167</v>
-      </c>
-      <c r="D40">
-        <v>162</v>
-      </c>
-      <c r="F40">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41">
-        <v>145</v>
-      </c>
-      <c r="F41">
-        <v>8.4600000000000009</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42">
-        <v>134</v>
-      </c>
-      <c r="F42">
-        <v>10.029999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43">
-        <v>130</v>
-      </c>
-      <c r="F43">
-        <v>11.56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>146</v>
-      </c>
-      <c r="B44">
-        <v>43</v>
-      </c>
-      <c r="C44" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44">
-        <v>127</v>
-      </c>
-      <c r="F44">
-        <v>13.08</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45">
-        <v>44</v>
-      </c>
-      <c r="C45" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45">
-        <v>125</v>
-      </c>
-      <c r="F45">
-        <v>14.59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>123</v>
       </c>
       <c r="D46">
         <v>125</v>
       </c>
-      <c r="F46">
+      <c r="E46">
+        <v>14.59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47">
+        <v>125</v>
+      </c>
+      <c r="E47">
         <v>16.16</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47">
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47">
+      <c r="C48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48">
         <v>128</v>
       </c>
-      <c r="F47">
+      <c r="E48">
         <v>17.66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>134</v>
-      </c>
-      <c r="E48">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="F48">
-        <v>19.21</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="B49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E49">
-        <v>3.38</v>
+        <v>19.21</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="B50">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E50">
-        <v>4.6900000000000004</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>24</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>25</v>
       </c>
       <c r="D51">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E51">
-        <v>5.94</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C52" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="D52">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E52">
-        <v>7.24</v>
+        <v>4.6900000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B53">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D53">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E53">
-        <v>8.59</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="B54">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="D54">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E54">
-        <v>9.9700000000000006</v>
+        <v>7.24</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B55">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D55">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E55">
-        <v>11.4</v>
+        <v>8.59</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B56">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D56">
-        <v>235</v>
+        <v>133</v>
+      </c>
+      <c r="E56">
+        <v>9.9700000000000006</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="B57">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D57">
-        <v>198</v>
+        <v>131</v>
+      </c>
+      <c r="E57">
+        <v>11.4</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B58">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D58">
-        <v>169</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B59">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D59">
-        <v>165</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="B60">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="D60">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>27</v>
       </c>
       <c r="D61">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B62">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D62">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="B63">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="D63">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="B64">
+        <v>61</v>
+      </c>
+      <c r="C64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66">
         <v>63</v>
       </c>
-      <c r="C64" t="s">
-        <v>45</v>
-      </c>
-      <c r="D64">
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66">
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65">
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67">
         <v>64</v>
       </c>
-      <c r="C65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D65">
+      <c r="C67" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66">
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68">
         <v>65</v>
       </c>
-      <c r="C66" t="s">
-        <v>145</v>
-      </c>
-      <c r="D66">
+      <c r="C68" t="s">
+        <v>142</v>
+      </c>
+      <c r="D68">
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69">
+        <v>66</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70">
+        <v>67</v>
+      </c>
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
         <v>40</v>
       </c>
-      <c r="B67">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68">
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69">
-        <v>68</v>
-      </c>
-      <c r="C69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69">
+      <c r="D71">
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>156</v>
-      </c>
-      <c r="B70">
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72">
         <v>69</v>
       </c>
-      <c r="C70" t="s">
-        <v>157</v>
-      </c>
-      <c r="D70">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>168</v>
-      </c>
-      <c r="B71">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>169</v>
-      </c>
-      <c r="D71">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72">
-        <v>71</v>
-      </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="D72">
         <v>156</v>
       </c>
-      <c r="F72">
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>165</v>
+      </c>
+      <c r="B73">
+        <v>70</v>
+      </c>
+      <c r="C73" t="s">
+        <v>166</v>
+      </c>
+      <c r="D73">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74">
+        <v>156</v>
+      </c>
+      <c r="E74">
         <v>6.62</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73">
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75">
         <v>72</v>
       </c>
-      <c r="C73" t="s">
-        <v>61</v>
-      </c>
-      <c r="D73">
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75">
         <v>144</v>
       </c>
-      <c r="F73">
+      <c r="E75">
         <v>8.14</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
-        <v>142</v>
-      </c>
-      <c r="B74">
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
-        <v>143</v>
-      </c>
-      <c r="D74">
+      <c r="C76" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76">
         <v>134</v>
       </c>
-      <c r="F74">
+      <c r="E76">
         <v>9.57</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" t="s">
-        <v>162</v>
-      </c>
-      <c r="B75">
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
-        <v>163</v>
-      </c>
-      <c r="D75">
+      <c r="C77" t="s">
+        <v>160</v>
+      </c>
+      <c r="D77">
         <v>130</v>
       </c>
-      <c r="F75">
+      <c r="E77">
         <v>10.96</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
-      <c r="A76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76">
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78">
         <v>75</v>
       </c>
-      <c r="C76" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76">
+      <c r="C78" t="s">
+        <v>118</v>
+      </c>
+      <c r="D78">
         <v>128</v>
       </c>
-      <c r="F76">
+      <c r="E78">
         <v>12.35</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77" t="s">
-        <v>102</v>
-      </c>
-      <c r="B77">
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79">
         <v>76</v>
       </c>
-      <c r="C77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D77">
+      <c r="C79" t="s">
+        <v>100</v>
+      </c>
+      <c r="D79">
         <v>126</v>
       </c>
-      <c r="F77">
+      <c r="E79">
         <v>13.73</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
-      <c r="A78" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78">
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80">
         <v>77</v>
       </c>
-      <c r="C78" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78">
+      <c r="C80" t="s">
+        <v>68</v>
+      </c>
+      <c r="D80">
         <v>127</v>
       </c>
-      <c r="F78">
+      <c r="E80">
         <v>15.13</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>116</v>
-      </c>
-      <c r="B79">
-        <v>78</v>
-      </c>
-      <c r="C79" t="s">
-        <v>117</v>
-      </c>
-      <c r="D79">
-        <v>130</v>
-      </c>
-      <c r="F79">
-        <v>16.55</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80">
-        <v>79</v>
-      </c>
-      <c r="C80" t="s">
-        <v>11</v>
-      </c>
-      <c r="D80">
-        <v>134</v>
-      </c>
-      <c r="E80">
-        <v>2.38</v>
-      </c>
-      <c r="F80">
-        <v>17.98</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="B81">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C81" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="D81">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E81">
-        <v>3.48</v>
+        <v>16.55</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="B82">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
       <c r="D82">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E82">
-        <v>4.6100000000000003</v>
+        <v>17.98</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>180</v>
       </c>
       <c r="B83">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="D83">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E83">
-        <v>5.77</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B84">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="D84">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E84">
-        <v>6.97</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B85">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="D85">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E85">
-        <v>8.19</v>
+        <v>4.6100000000000003</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="B86">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D86">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E86">
-        <v>9.44</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="B87">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="D87">
-        <v>165</v>
+        <v>146</v>
+      </c>
+      <c r="E87">
+        <v>6.97</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="B88">
+        <v>84</v>
+      </c>
+      <c r="C88" t="s">
+        <v>110</v>
+      </c>
+      <c r="D88">
+        <v>146</v>
+      </c>
+      <c r="E88">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89">
+        <v>85</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89">
+        <v>145</v>
+      </c>
+      <c r="E89">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>147</v>
+      </c>
+      <c r="B90">
+        <v>90</v>
+      </c>
+      <c r="C90" t="s">
+        <v>148</v>
+      </c>
+      <c r="D90">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>155</v>
+      </c>
+      <c r="B91">
         <v>92</v>
       </c>
-      <c r="C88" t="s">
-        <v>159</v>
-      </c>
-      <c r="D88">
+      <c r="C91" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91">
         <v>142</v>
       </c>
     </row>

</xml_diff>